<commit_message>
Slimmed down report w/ security hotspots to provide as artifact.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -5,74 +5,25 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amthomas/dev/testing/en-report/sonar-cnes-report/src/main/resources/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amthomas/dev/testing/sonar-cnes-report/src/main/resources/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5837C2-E85B-4E48-A3C9-8DD61C0DCCF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC2E960-0552-D448-852B-BFA288EC4AC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="520" windowWidth="19880" windowHeight="12560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="2040" windowWidth="21060" windowHeight="13460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TCD" sheetId="3" r:id="rId1"/>
-    <sheet name="Issues" sheetId="1" r:id="rId2"/>
-    <sheet name="All" sheetId="2" r:id="rId3"/>
-    <sheet name="Unconfirmed" sheetId="4" r:id="rId4"/>
-    <sheet name="Hotspots" sheetId="6" r:id="rId5"/>
-    <sheet name="Metrics" sheetId="5" r:id="rId6"/>
+    <sheet name="ISSUES" sheetId="2" r:id="rId1"/>
+    <sheet name="HOTSPOTS" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <pivotCaches>
-    <pivotCache cacheId="79" r:id="rId7"/>
-  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
-  <si>
-    <t>Rule</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>Nombre de Message</t>
-  </si>
-  <si>
-    <t>Effort</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>Colonne1</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>(blank)</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -557,28 +508,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -625,24 +558,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="2">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -660,209 +578,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Aaron Thomas" refreshedDate="43972.002707754633" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF07000000}">
-  <cacheSource type="worksheet">
-    <worksheetSource name="selected"/>
-  </cacheSource>
-  <cacheFields count="10">
-    <cacheField name="Rule" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="6">
-        <m/>
-        <s v="python:FunctionComplexity" u="1"/>
-        <s v="python:S1066" u="1"/>
-        <s v="python:S134" u="1"/>
-        <s v="python:S107" u="1"/>
-        <s v="python:S125" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Message" numFmtId="4">
-      <sharedItems containsNonDate="0" containsBlank="1" count="7">
-        <m/>
-        <s v="Remove this commented out code." u="1"/>
-        <s v="Function has a complexity of 11 which is greater than 10 authorized." u="1"/>
-        <s v="Function has a complexity of 47 which is greater than 10 authorized." u="1"/>
-        <s v="Function &quot;generate_spaceship&quot; has 11 parameters, which is greater than the 7 authorized." u="1"/>
-        <s v="Refactor this code to not nest more than 3 &quot;if&quot;, &quot;for&quot;, &quot;while&quot;, &quot;try&quot; and &quot;with&quot; statements." u="1"/>
-        <s v="Merge this if statement with the enclosing one." u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Type" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="2">
-        <m/>
-        <s v="CODE_SMELL" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Severity" numFmtId="0">
-      <sharedItems containsNonDate="0" containsBlank="1" count="2">
-        <m/>
-        <s v="MAJOR" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Language" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="File" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Line" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Effort" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Status" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Comments" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="synthesis" cacheId="79" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item m="1" x="1"/>
-        <item m="1" x="2"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="8">
-        <item m="1" x="4"/>
-        <item m="1" x="2"/>
-        <item m="1" x="3"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="1">
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="5">
-    <field x="4"/>
-    <field x="2"/>
-    <field x="3"/>
-    <field x="0"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x v="5"/>
-    </i>
-    <i r="4">
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Nombre de Message" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rule"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Message" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Severity"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Language"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="File"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Line"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Effort"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Status"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Comments"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="issues" displayName="issues" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Colonne1"/>
@@ -871,40 +588,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Rule"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Message" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Severity"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Language"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="File"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Line"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Effort"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Status"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Comments"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7C0E2B34-BAF6-6345-88D7-2F6A226ECE53}" name="hotspots" displayName="hotspots" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D4D36166-C0B9-0B4E-A8F1-FAD58A975208}" name="hotspots" displayName="hotspots" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{13BEF51C-EF80-264A-8DDE-E3150A0A8CC2}" name="Colonne1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="metrics" displayName="metrics" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Colonne1"/>
+    <tableColumn id="1" xr3:uid="{7E195CDB-4C4C-D740-96AE-EDECDB7DC45F}" name="Colonne1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1230,264 +918,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="pivotTable"/>
-  <dimension ref="A3:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="selectedIssues"/>
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="63.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="allIssues"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="63.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A53885-0649-3F4C-8935-9B0FEA133949}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1502,9 +934,41 @@
     <col min="16" max="16" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C159C67-05F3-D54B-86B8-AF6B15928A19}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>